<commit_message>
Many tests added and bugs fixed.
Just before major changes to _applyExactConversionDirectives and _applyRegexConversionDirectives. Need to change how isUnique works.
</commit_message>
<xml_diff>
--- a/tests/testing_files/child_tag_example.xlsx
+++ b/tests/testing_files/child_tag_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparda\Desktop\Moseley Lab\Code\MESSES\tests\testing_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088AC76C-54E0-4FE3-A38A-7A60355CC891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF1AD3F-3B8F-445D-B541-F526A0ABDBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="1665" windowWidth="23565" windowHeight="12015" xr2:uid="{74622A20-6192-4670-9736-88E18B0F4086}"/>
+    <workbookView xWindow="3120" yWindow="1830" windowWidth="23640" windowHeight="12015" xr2:uid="{74622A20-6192-4670-9736-88E18B0F4086}"/>
   </bookViews>
   <sheets>
     <sheet name="#export" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>